<commit_message>
forgot 2 more sheets
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osten\loCalendar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6897F7-C9BC-4D16-AF3E-2B396420D25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10386740-30AE-45EC-B3F7-8DF8058A0DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{A6D4DD5A-4642-4146-9CF1-87147E748D5C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="2" xr2:uid="{A6D4DD5A-4642-4146-9CF1-87147E748D5C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="10" sheetId="1" r:id="rId1"/>
+    <sheet name="100" sheetId="2" r:id="rId2"/>
+    <sheet name="1000" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="14">
   <si>
     <t>First</t>
   </si>
@@ -429,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BAFABCB-B013-4245-BF63-613FBFCF1254}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="A1:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -606,4 +608,362 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10FB320D-C578-4CA1-BCE7-47B5E47FC8FF}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="e">
+        <f>AVERAGE(B3:F3)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="e">
+        <f t="shared" ref="G4:G9" si="0">AVERAGE(B4:F4)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" t="e">
+        <f>AVERAGE(B12:F12)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" t="e">
+        <f t="shared" ref="G13:G17" si="1">AVERAGE(B13:F13)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{866543AA-C5E3-4D95-AD05-1451F0DDEC40}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="e">
+        <f>AVERAGE(B3:F3)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="e">
+        <f t="shared" ref="G4:G9" si="0">AVERAGE(B4:F4)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" t="e">
+        <f>AVERAGE(B12:F12)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" t="e">
+        <f t="shared" ref="G13:G17" si="1">AVERAGE(B13:F13)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>